<commit_message>
ajuste historias de usuario, mock up empleado
</commit_message>
<xml_diff>
--- a/Documentacion/Historias de usuario.xlsx
+++ b/Documentacion/Historias de usuario.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Hoja 1'!$B$2:$J$62</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Hoja 1'!$A$2:$J$74</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="351">
   <si>
     <t>Enunciado de la historia</t>
   </si>
@@ -51,16 +51,13 @@
     <t>Resultado/Comportamiento esperado</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>Recursos humanos</t>
   </si>
   <si>
     <t>Contrato</t>
   </si>
   <si>
-    <t>El usuario al entrar al modulo vera por medio de un listado con paginacion todos los contratos que estan en estado firmados, faltantes por firmar, y pendientes por validacion(esto por bandejas) tambien este listado se va a manejar por filtros, se van a poder ver los campos: Radicado, estado del contrato, titulo, fecha creacion, fecha firma(si esta en estado firmado)</t>
+    <t>Ver un listado de los contratos, mostrando informacion relevante a primera vista</t>
   </si>
   <si>
     <t>Para un mayor control del almacenamiento de los contratos</t>
@@ -90,7 +87,7 @@
     <t>Filtrar por el texto que se haya escrito en el buscador</t>
   </si>
   <si>
-    <t>Al momento de darle click al boton de crear que estara ubicado en la parte superior del listado principal, se va a desplegar un formulario con los campos, partes implicadas(InputSelectMultiple), titulo del contrato(TextField), categoria de contrato(inputSelect), tipo de contrato(input select), es persona externa?(check), cuerpo normatio(textField), fecha terminacion del contrato(DatePicker), forma de cierre del contrato(TextField). correo del implicado externo(esto en caso de que si es persona extena esta chequeado).</t>
+    <t>Generar un nuevo contrato.</t>
   </si>
   <si>
     <t>Se guardara con estado "Por Verificar", al momento de darle click a guardar contrato, esto para que luego se pase a revision.</t>
@@ -138,8 +135,7 @@
     <t>Peticiones/Solicitudes</t>
   </si>
   <si>
-    <t xml:space="preserve">El sistema permitirá a los empleados crear nuevas peticiones de diferentes tipos según sus necesidades, categorizandolas en prestamos, peticiones inasistencias, recursos, capacitaciones, relacionadas al puesto, reclamos.
-</t>
+    <t>El sistema permitirá a los empleados crear nuevas peticiones de diferentes tipos según sus necesidades y su categoria.</t>
   </si>
   <si>
     <t>Permite al usuario crear su peticion deacuerdo a su necesidad</t>
@@ -160,7 +156,7 @@
     <t>Jefe de Area</t>
   </si>
   <si>
-    <t>El usuario podra ingresar al modulo de solicitudes, donde por su permiso solo va a poder ver un listado de peticiones que esten dentro de la categoria "inasistencias", donde ademas de este filtro, va a poder solo ver las que fueron creadas por aquellos empleados que pertenecen a su area, puede ver los diferentes filtros que le puede aplicar a la tabla.</t>
+    <t>El usuario al entrar al modulo, segun su permiso solo va a poder ver las solicitudes que esten dentro de la categoria de inasistencias</t>
   </si>
   <si>
     <t>Con la finalidad de que el usuario pueda ver que usuarios dentro de su area no pueden asistir el dia de la consulta, junto su motivo.</t>
@@ -181,7 +177,7 @@
     <t>Postulado</t>
   </si>
   <si>
-    <t>Luego de que el contrato pase de estado "por revisar" a "aprovado", al usuario externo, si aplica, le va a llegar una notificacion al correo donde se le va a proporcionar un link donde el usuario puede acceder al contrato, validar los terminos de este, siempre y cuando este dentro del plazo pre definido</t>
+    <t>Ver el contrato y hacer validaciones, esto para pasar a firmarlo.</t>
   </si>
   <si>
     <t>Con la finalidad de que el usuario externo que hace parte de los involucrados que deben firmarlo</t>
@@ -211,7 +207,7 @@
     <t>Cuando alguno de los involucrados hayan subido sus incorfomidades este contrato pasara de estado "aprovado" a "Devuelto por Involucrados", esto para que se revise otra vez y se vueva a reiniciar el proceso.</t>
   </si>
   <si>
-    <t>En el momento en el cual a un contrato llegue a la fecha de vencimiento, el contrato debera establecerse en un estado de "vencido", esto automanticamente por medio de un trigger(el trigger tambien deshabilitara al empleado del sistema), cuando el usuario entra al detalle de este contrato vencido tiene la opcion de renovar contrato o dar por finalizado este.</t>
+    <t>Cuando el contrato esta vencido, el usuario tiene la opcion de renovar el contrato.</t>
   </si>
   <si>
     <t>Esto para finalizar definitivamente el flujo del contrato o renovar creando una copia del contrato, estableciendolo a estado "por revisar"</t>
@@ -307,10 +303,10 @@
     <t>Se podra ver un listado de todos los movimientos hechos referentes al contrato.</t>
   </si>
   <si>
-    <t>El usuario tiene la capacidad de eliminar la solicitud que ya genero solo en caso de que aun este en estado pendiente. En otras palabras, aun no ha sido revisada por el jefe o recursos humanos</t>
-  </si>
-  <si>
-    <t>Realizar la cancelacion y/o eliminacion de la solicitud</t>
+    <t>Eliminar solicitud</t>
+  </si>
+  <si>
+    <t>Realizar la cancelacion y/o eliminacion de la solicitud, solo si no ha sido revisada.</t>
   </si>
   <si>
     <t>Eliminar la solicitud</t>
@@ -325,10 +321,10 @@
     <t>Al confirmar la eliminacion se realizara el proceso</t>
   </si>
   <si>
-    <t>El usuario tiene la capacidad de editar la solicitud que ya genero solo en caso de que aun este en estado pendiente. En otras palabras, aun no ha sido revisada por el jefe o recursos humanos</t>
-  </si>
-  <si>
-    <t>Editar la solicitud para cambiar una fecha o un documento incorrecto</t>
+    <t>Editar la solicitud</t>
+  </si>
+  <si>
+    <t>Editar la solicitud, solo si no ha sido revisada.</t>
   </si>
   <si>
     <t>Editar la solicitud para modificar la fecha de vacaciones</t>
@@ -352,10 +348,10 @@
     <t>Jefe de area</t>
   </si>
   <si>
-    <t>El usuario tiene la capacidad de aprovar o rechazar alguna de estas peticiones, esto para notificarle al empleado quien crea la peticion de su estado, si es aprovada o rechazada.</t>
-  </si>
-  <si>
-    <t>Para mostrar su conformidad al empleado.</t>
+    <t>Aprovar o rechazar solicitud o peticion</t>
+  </si>
+  <si>
+    <t>Para notificar al peticionario sobre la descicion acerca de la peticion</t>
   </si>
   <si>
     <t>Aprovar peticion.</t>
@@ -385,20 +381,19 @@
     <t>Recursos Humanos</t>
   </si>
   <si>
-    <t>El usuario podra ingresar al modulo de solicitudes, va a poder ver absolutamente todas las peticiones, puede ver los diferentes filtros que le puede aplicar a la tabla.</t>
+    <t>Listado de peticiones y sus filtros.</t>
   </si>
   <si>
     <t>Con la finalidad de que el usuario de recursos humanos este al tanto de las peticiones que se han hecho, esto haciendo caso a los filtros que puede aplicar</t>
   </si>
   <si>
-    <t>El usuario podra ingresar al modulo de solicitudes, va a poder solo ver las que fueron creados por si mismo, puede ver los diferentes filtros que le puede aplicar a la tabla.</t>
+    <t>Ver las peticiones creadas por el usuario</t>
   </si>
   <si>
     <t>El usuario puede filtrar las solicitudes, ya sea por el titulo, categoria, estado, tipo.</t>
   </si>
   <si>
-    <t xml:space="preserve">El sistema permitirá al usuario crear nuevas peticiones de diferentes tipos según sus necesidades, categorizandolas en prestamos, peticiones inasistencias, recursos, capacitaciones, relacionadas al puesto, reclamos.
-</t>
+    <t>Crear peticiones y solicitudes segun categoria y tipo.</t>
   </si>
   <si>
     <t>Jefe de area-recursos humanos</t>
@@ -407,10 +402,10 @@
     <t>Vacantes</t>
   </si>
   <si>
-    <t>Al momento de entrar al modulo, el usuario va a ver el listado de todos las vacantes, tambien va a ver bandejas (aprovadas, rechazadas, terminadas, por publicar), viendo los campos de cada una: Radicado, estado, fecha creacion y cantidad de aplicantes, dividiendolos por paginacion</t>
-  </si>
-  <si>
-    <t>Para poder visualizar las vacantes</t>
+    <t>Ver listado de vacantes junto sus filtros</t>
+  </si>
+  <si>
+    <t>Para poder visualizar las vacantes actuales, podiendo filtrar por su estado y demas campos</t>
   </si>
   <si>
     <t>Filtrar las vacantes</t>
@@ -422,22 +417,28 @@
     <t>Desea hacer una busqueda ya sea por el titulo del vacantes o su radicado</t>
   </si>
   <si>
-    <t>Al momento de entrar al aplicativo va a ver la opcion de "trabaja con nosotros", donde el usuarios, al darle click, se va a redirigir a otra ventana, donde el usuario va a poder seleccionar el cargo (si esta disponible) en el que quiere trabajar para la empresa.</t>
-  </si>
-  <si>
-    <t>Para mostrarle al usuario las vacantes disponibles para ese cargo, en este listado se van a mostrar los campos, titulo vacante, salario, frecuencia de pago, y el boton de aplicar.</t>
-  </si>
-  <si>
-    <t>Al momento de que el usuario dentro del listado de vacantes al que ya entro, tiene la opcion de darle click a "aplicar a vacante"</t>
-  </si>
-  <si>
-    <t>Para que se rediriga al usuario al formulario que va a tener los campos: foto de aplicante, nombres, apellidos, direccion, correo, telefono de contacto, fecha de nacimiento, caracteristicas del aplicante, informacion academica, experiencia laboral, un campo ademas de esto, donde se pueda poner informacion adicional si asi lo desea, tambien debera aceptar el habeas data(acepta la trata de informacion, requerido por ley).</t>
+    <t>Listado de vacantes disponibles a las que aplciar, junto sus filtros</t>
+  </si>
+  <si>
+    <t>Mostrar al usuario las vacantes que fueron previamente publicados por rh, para mas tarde aplicar a alguna o previsualizarla.</t>
+  </si>
+  <si>
+    <t>Aplicar a la vacante.</t>
+  </si>
+  <si>
+    <t>Para que el usuario aplique a la vacante que le parece de acuerdo a sus capacidades.</t>
   </si>
   <si>
     <t>Desee aplicar</t>
   </si>
   <si>
-    <t>Darle al boton de guardar, esto subira su hoja de vida a nuestra base de datos.</t>
+    <t>Si quiere aplicar a la vacante seleccionada</t>
+  </si>
+  <si>
+    <t>Al darle click al boton de aplicar, se abrira un dialog de confirmacion.</t>
+  </si>
+  <si>
+    <t>Cuando el usuario confirme, se adjuntara su hoja de vida a la vacante.</t>
   </si>
   <si>
     <t>No desee aplicar</t>
@@ -446,7 +447,13 @@
     <t>Darle al boton de cancelar aplicacion, esto lo devolva a la pagina inicial.</t>
   </si>
   <si>
-    <t>Al momento de que el usuario quiera ver o manipular informacion principal de la vacante.</t>
+    <t>Si el usuario ya no quiere hacer una aplicacion labora</t>
+  </si>
+  <si>
+    <t>El podra cerrar el modal.</t>
+  </si>
+  <si>
+    <t>Ver o manipular informacion principal de la vacante.</t>
   </si>
   <si>
     <t>Para ver la informacion general de la vacante, en esta vista vamos a poder ver dos principales tabs, detalle de la vacante, y aplicantes, donde en aplicantes va a poder validar las hojas de vida de cada uno de estos y incluso eliminar registros, esto por si algun usuario externo subio informacion irrelebante o inapropiada.</t>
@@ -530,7 +537,7 @@
     <t>Reportes</t>
   </si>
   <si>
-    <t>El usuario al momento de ingresar al modulo de reportes vera los reportes posibles segun los modulos del aplicativo por medio de tarjetas interactivas, aplicando filtros de lo que desee ver puntualmente en el modal que la tarjeta ejecuta.</t>
+    <t>Desea generar un reporte</t>
   </si>
   <si>
     <t>El modulo le dejaria una facil organizacion para consultar algun informe e informacion generalizada, descargando un archivo excel trayendo la informacion que vienen de los filtros.</t>
@@ -548,6 +555,18 @@
     <t>Al momento de darle click al boton de generar, se descargara un archivo excel de la informacion compilada.</t>
   </si>
   <si>
+    <t>Ver todos los aplicantes</t>
+  </si>
+  <si>
+    <t>Al momento de darle ver todos los aplicantes, se traera un listado, de todos los postulados que han aplicado a la vacante</t>
+  </si>
+  <si>
+    <t>Al momento de darle dentro de las opciones de la vacante, al boton de ver aplicantes, mostrando un listado de los aplicantes, teniendo la opcion de ver la hoja de vida.</t>
+  </si>
+  <si>
+    <t>Al darle al boton de ver la hoja de vida, se ampliara una vista y se mostrar la hoja  de vida generada como un pdf</t>
+  </si>
+  <si>
     <t>Archivar aplicante</t>
   </si>
   <si>
@@ -578,7 +597,7 @@
     <t>Horario</t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario ingresa al modulo para consultar los horarios que estan diponibles en su area, puede ver los campos del dia 'inicio y final', 'hora inicio y finalizacion de la jornada'. </t>
+    <t>Ver listado de horarios que tengo en mi area, junto los filtros correspondientes.</t>
   </si>
   <si>
     <t>Con el fin de ver todos los horarios que tiene sus empleados del area.</t>
@@ -629,7 +648,7 @@
     <t>Comunicados Internos</t>
   </si>
   <si>
-    <t>Este sera tomado como la pagina inicial, donde el usuario va a poder ver los comunicados que han creado los usuarios de recursos humanos, junto a estos post una pequeña vista para mostrar a los empleados que hoy cumplen años.Los campos que se van a mostrarse en el listado de comunicados, van a ser fotos del post, descripcion, like y dislike. Al darle click al post se ampleara el post mostando todas las imagenes y mostrando el post a mas detalle.</t>
+    <t>Ver los comunicados actuales.</t>
   </si>
   <si>
     <t>El usuario de esta forma se enterara de los eventos principales que se estan organizando, puede reaccionar por medio de likes o dislikes.</t>
@@ -671,9 +690,6 @@
     <t>Al darle guardar reporte, se subira a la base de datos y se le notificara al usuario que posteo el comunicado esta incorformidad por medio de un correo electronico.</t>
   </si>
   <si>
-    <t>Este sera tomado como la pagina inicial, donde el usuario va a poder ver los comunicados que han creado los usuarios de recursos humanos, junto a estos post una pequeña vista para mostrar a los empleados que hoy cumplen años.Los campos que se van a mostrarse, van a ser fotos del post, descripcion, like, dislikes y reportes. Al darle click al post se ampleara el post mostando todas las imagenes y mostrando el post a mas detalle.</t>
-  </si>
-  <si>
     <t>El usuario de esta forma se enterara de los eventos principales que se estan organizandos, puede reaccionar por medio de likes o dislikes, y los reportes que se les subieron a este.</t>
   </si>
   <si>
@@ -701,22 +717,46 @@
     <t>Se mostrara un formulario de edicion donde se mostrara los campos con los datos actuales. Los campos son titulo, decripcion, anexar fotos.</t>
   </si>
   <si>
-    <t>Si el empleado llega a tener complicaciones para asistir a un dia de jornada laboral, puede mostrar una excusa que valide su falta</t>
-  </si>
-  <si>
-    <t>Con el fin de no generar un reporte para el empleado, este tiene la capacidad de mostrar una excusa que valide su falla</t>
-  </si>
-  <si>
-    <t>El usuario presenta alguna excusa para evitar un reporte</t>
-  </si>
-  <si>
-    <t>Al momento de que el usuario no pueda cumplir con el horario.</t>
-  </si>
-  <si>
-    <t>Tras ingresar al registro de su horario, se da click en la opcion de generar excusa la cual sera posteriormente revisada y validada</t>
-  </si>
-  <si>
-    <t>Se guardara su excusa en el modulo de peticiones/solicitudes, guardandola dentro de la categoria "incapacidades", y de ahi empezaria el flujo de peticiones/solicitudes</t>
+    <t>Ver horarios asignados</t>
+  </si>
+  <si>
+    <t>Con el fin de que el responsable del horario se entere de las acciones de su empleado dentro del horario esto por medio de ciertas acciones. que estan disponibles dentro del menu</t>
+  </si>
+  <si>
+    <t>Crear una incapacidad</t>
+  </si>
+  <si>
+    <t>Al momento de que el usuario no pueda cumplir con el horario, y tenga una excusa justificada</t>
+  </si>
+  <si>
+    <t>Tras ingresar al registro de su horario, se da click al menu de opciones, luego al boton de incapacidad, se abrira un formulario el cual debe llenar completamente, seleccionando el tipo de incapacidad, dandole un titulo y su justificacion, tambien tiene la opcion de subir un comprobante.</t>
+  </si>
+  <si>
+    <t>Al darle a guardar, se guardara adjunto a la informacion del horario, esto para que pase a revision mas adelante por cualquier usuario con permisos para esto</t>
+  </si>
+  <si>
+    <t>Solicitar.</t>
+  </si>
+  <si>
+    <t>Al momento de que el usuario quiera hacer una solicitud, por ejemplo, solicitar vacaciones o cambio de horario.</t>
+  </si>
+  <si>
+    <t>Tras ingresar al registro de su horario, se da click al menu de opciones, luego al boton de solicitar, se abrira un formulario el cual debe llenar completamente, seleccionando el tipo de solicitud, dandole un titulo y su justificacion.</t>
+  </si>
+  <si>
+    <t>Al darle a guardar, primero se guardara en el modulo de solicitudes, y tambien se guardara adjunto a la informacion del horario informacion basica con un hypervinculo para acceder luego.</t>
+  </si>
+  <si>
+    <t>Horas Extra</t>
+  </si>
+  <si>
+    <t>Al momento de que, si el usuario hizo horas extras.</t>
+  </si>
+  <si>
+    <t>Tras ingresar al registro de su horario, se da click al menu de opciones, luego al boton de extras, se abrira un formulario el cual debe llenar completamente,dandole un titulo, cantidad de horas y su justificacion.</t>
+  </si>
+  <si>
+    <t>Al darle a guardar, se guardara adjunto a la informacion del horario.</t>
   </si>
   <si>
     <t>Recursos humanos/Jefe de area</t>
@@ -725,7 +765,7 @@
     <t>Comunicados internos</t>
   </si>
   <si>
-    <t>El usuario al crear un comunicado debera llenar un formulario el cual va a contener: Titulo, descripcion, anexo de fotos.</t>
+    <t>Crear comunicado.</t>
   </si>
   <si>
     <t>Con el fin de hacer una publicacion en comunicados.</t>
@@ -743,7 +783,7 @@
     <t>Se registrara en la tabla de comunicados en la db, cerrando el formulario.</t>
   </si>
   <si>
-    <t>Recursos humanos verifica la excusa presentada por el empleado y modificando su estado para aceptarla o rechzarla.</t>
+    <t>Verificar excusa.</t>
   </si>
   <si>
     <t>Con la finalidad de actualizar el estado de la excusa</t>
@@ -779,13 +819,13 @@
     <t>Permite que Recursos Humanos se entere de su ingreso y salida</t>
   </si>
   <si>
-    <t>El usuario al momento de entrar al modulo, vera el listado de los horarios donde este ha sido mensionado por su jefe en area</t>
+    <t>Listado de horarios asignados, junto el filtro</t>
   </si>
   <si>
     <t>Con la finalidad de que el usuario este al tanto de sus horarios</t>
   </si>
   <si>
-    <t>El usuario necesita generar algun reporte de que un usuario no se ha presentado a trabajar y no ha generado ninguna incapacidad dentro del modulo de peticiones/solicitudes</t>
+    <t>Generar una incapacidad.</t>
   </si>
   <si>
     <t>Con la finalidad de que el usuario pueda reportar a recursos humanos alguna irregularidad de algun empleado</t>
@@ -807,7 +847,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario va a poder ver el listado de empleados, dando click seleccionando al que desea ver, desplegandose una ventana donde puede visualizar ese perfil con la informacion del empleado donde tambien incluye papeles importantes que puedan necesitar los empleados.  </t>
+    <t>Visualizar empleado.</t>
   </si>
   <si>
     <t>Facilitar la gestion de informacion del empleado para la facil accesibilidad a papeles que puedan se puedan necestar.</t>
@@ -837,7 +877,7 @@
     <t>Tendra la descripcion del porque se requiere este campo y en que campo, y por ultimo se hara la edicion</t>
   </si>
   <si>
-    <t>ver su informacion principal junto a papeles que pueda necesitar, teniendo esto en el mismo perfil ayudando a la accesibilidad</t>
+    <t>Ver informacion personal</t>
   </si>
   <si>
     <t>cada empleado tiene imformacion necesaria a la mano</t>
@@ -873,7 +913,7 @@
     <t xml:space="preserve">Imformacion de Empleados </t>
   </si>
   <si>
-    <t>EL usuario va a poder modificar los permisos y roles existentes en el aplicativo, por medio de una sencilla interfas</t>
+    <t>Gestion de roles y permisos.</t>
   </si>
   <si>
     <t>Para administrar de forma eficiente los usuarios que puedan gestionar ciertos modulos.</t>
@@ -901,6 +941,132 @@
   </si>
   <si>
     <t>Al momento de darle al checkbox, se va a eliminar este permiso para el rol.</t>
+  </si>
+  <si>
+    <t>Comunicados</t>
+  </si>
+  <si>
+    <t>Gestionar comunicados.</t>
+  </si>
+  <si>
+    <t>Para mayor control por parte del usuario cumpliendo con los requerimientos que requiere el rol</t>
+  </si>
+  <si>
+    <t>Crear comunicado</t>
+  </si>
+  <si>
+    <t>Por si el usuario quiere crear un nuevo comunicado</t>
+  </si>
+  <si>
+    <t>Al momento de darle al boton de crear se desplegara el formulario correspondiente al modulo</t>
+  </si>
+  <si>
+    <t>Al darle a publciar se guardara y se mostrara a los otros usuarios</t>
+  </si>
+  <si>
+    <t>Editar comunicado</t>
+  </si>
+  <si>
+    <t>Por si el usuario quiere editar el comunicado.</t>
+  </si>
+  <si>
+    <t>Dentro del menu de opciones, el usuario tiene la capacidad de hacer ciertas acciones, entre esas acciones, el podra editar el cominicado</t>
+  </si>
+  <si>
+    <t>Al momento de darle actualizar, el comunicado se guardara, y se actualizara a los damas usuarios.</t>
+  </si>
+  <si>
+    <t>Eliminar comunicado</t>
+  </si>
+  <si>
+    <t>Por si el usuario quiere eliminar el comunicado</t>
+  </si>
+  <si>
+    <t>Dentro del menu de opciones, el usuario tiene la capacidad de hacer ciertas acciones, entre esas acciones, el podra eliminar el cominicado</t>
+  </si>
+  <si>
+    <t>Al momento de hacer la confirmacion, el cambio se guardara, y se actualizara el listado principal.</t>
+  </si>
+  <si>
+    <t>Infornacion de empleados.</t>
+  </si>
+  <si>
+    <t>Crear, eliminar, modificar usuarios junto a su informacion.</t>
+  </si>
+  <si>
+    <t>Para administrar de formac eficiente los usuarios y tener un mayor control sobre esta informacion</t>
+  </si>
+  <si>
+    <t>Ver todos los usuarios</t>
+  </si>
+  <si>
+    <t>Al entrar a este apartado vera el listado de todos los usuarios, en primera vista, vera la informacion como lo son: Nombres, Rol, Cargo, Estado, Correo y Tiene CV(esto para mostrar si tiene una hoja de vida cargada), tambien mostrara los posibles filtros que se pueden aplicar para el listado</t>
+  </si>
+  <si>
+    <t>Al darle al boton del filtrar, se mostraran los posibles filtros,</t>
+  </si>
+  <si>
+    <t>Al seleccionar los filtros se recargara el listado, aplicando los filtros en el listado y su paginado.</t>
+  </si>
+  <si>
+    <t>Crear usuario</t>
+  </si>
+  <si>
+    <t>Por si se requiere un usuario nuevo</t>
+  </si>
+  <si>
+    <t>Al darle al boton de crear, el usuario vera un formulario, el cual es similar al crear una hoja de vida, donde la mayoria de la informacion es opcional a llenar.</t>
+  </si>
+  <si>
+    <t>Al momento de darle al boton de crear, se guardara el usuario, si se selecciono un puesto para el usuario, se creara directamente con rol empleado, pero si no se creara como postulado, aunque su rol puede ser opcional.</t>
+  </si>
+  <si>
+    <t>Ver informacion</t>
+  </si>
+  <si>
+    <t>Al momento de que se quiera ver la informacion del usuario</t>
+  </si>
+  <si>
+    <t>Al momento de darle al nombre del usuario en el listado de usuarios, este abrira una ventanita con la informacion del uisuario, junto todas sus aciones posibles</t>
+  </si>
+  <si>
+    <t>Esto le mostrara toda la informacion actual del usuario seleccionado</t>
+  </si>
+  <si>
+    <t>Editar usuario</t>
+  </si>
+  <si>
+    <t>Por si se inserto informacion errona, o simplemente desea actualizar cierta informacion.</t>
+  </si>
+  <si>
+    <t>Al darle al boton de editar, el usuario vera un formulario, el cual es similar al editaruna hoja de vida, aqui estara la informacion a cambiar, donde la mayoria de la informacion es opcional a llenar.</t>
+  </si>
+  <si>
+    <t>Al momento de darle, guardar cambios, habra una recarga de la informacion del usuario actuarl.</t>
+  </si>
+  <si>
+    <t>Cambiar rol</t>
+  </si>
+  <si>
+    <t>Por si se desea ascender a un usuario segun su rol</t>
+  </si>
+  <si>
+    <t>Al darle al boton reasignar rol, el usuario vera un formulario, mostrando los roles existentes</t>
+  </si>
+  <si>
+    <t>Al darle al guardar, se acualizara la informacion del usuario.</t>
+  </si>
+  <si>
+    <t>Desactivar usuario</t>
+  </si>
+  <si>
+    <t>Por si se requiere bloquear el acceso del aplicativo a usuario seleccionado</t>
+  </si>
+  <si>
+    <t>Al momento de darle al boton de desactivar.Al memento de darle al switch simple que estara como una opcion</t>
+  </si>
+  <si>
+    <t>Se actualizara la informacion desactivando al usuario.</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1177,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1315,35 +1481,35 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" ht="78.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="F3" s="4">
         <v>1.0</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1367,16 +1533,16 @@
         <v>2.0</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1400,31 +1566,31 @@
         <v>2.0</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="F5" s="4">
         <v>1.0</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1448,16 +1614,16 @@
         <v>2.0</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1481,16 +1647,16 @@
         <v>3.0</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1514,31 +1680,31 @@
         <v>3.0</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="F8" s="4">
         <v>1.0</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1562,31 +1728,31 @@
         <v>4.0</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="F9" s="4">
         <v>1.0</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1610,31 +1776,31 @@
         <v>5.0</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="F10" s="4">
         <v>1.0</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="I10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1658,16 +1824,16 @@
         <v>2.0</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1691,31 +1857,31 @@
         <v>6.0</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="D12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="F12" s="4">
         <v>1.0</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1739,16 +1905,16 @@
         <v>2.0</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1768,32 +1934,35 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
+      <c r="A14" s="4">
+        <v>7.0</v>
+      </c>
       <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="F14" s="4">
         <v>1.0</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1813,23 +1982,20 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="4">
-        <v>4.0</v>
-      </c>
       <c r="F15" s="4">
         <v>2.0</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1853,16 +2019,16 @@
         <v>3.0</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1886,16 +2052,16 @@
         <v>4.0</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="J17" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1919,16 +2085,16 @@
         <v>5.0</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1948,32 +2114,35 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" ht="60.0" customHeight="1">
+      <c r="A19" s="4">
+        <v>8.0</v>
+      </c>
       <c r="B19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="F19" s="4">
         <v>1.0</v>
       </c>
       <c r="G19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1993,32 +2162,35 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
+      <c r="A20" s="4">
+        <v>9.0</v>
+      </c>
       <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="F20" s="4">
         <v>1.0</v>
       </c>
       <c r="G20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -2038,17 +2210,14 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21">
-      <c r="A21" s="4">
-        <v>7.0</v>
-      </c>
       <c r="F21" s="4">
         <v>2.0</v>
       </c>
       <c r="G21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -2069,34 +2238,34 @@
     </row>
     <row r="22">
       <c r="A22" s="4">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="F22" s="4">
         <v>1.0</v>
       </c>
       <c r="G22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="J22" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -2120,16 +2289,16 @@
         <v>2.0</v>
       </c>
       <c r="G23" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="J23" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -2150,34 +2319,34 @@
     </row>
     <row r="24">
       <c r="A24" s="4">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="F24" s="4">
         <v>1.0</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -2198,34 +2367,34 @@
     </row>
     <row r="25">
       <c r="A25" s="4">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F25" s="4">
         <v>1.0</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -2246,34 +2415,34 @@
     </row>
     <row r="26">
       <c r="A26" s="4">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="4">
         <v>1.0</v>
       </c>
       <c r="G26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -2294,34 +2463,34 @@
     </row>
     <row r="27">
       <c r="A27" s="4">
-        <v>9.0</v>
+        <v>14.0</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="F27" s="4">
         <v>1.0</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -2345,16 +2514,16 @@
         <v>2.0</v>
       </c>
       <c r="G28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="I28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2375,19 +2544,19 @@
     </row>
     <row r="29">
       <c r="A29" s="4">
-        <v>10.0</v>
+        <v>15.0</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -2413,31 +2582,35 @@
     </row>
     <row r="30">
       <c r="A30" s="4">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="F30" s="4">
         <v>1.0</v>
       </c>
       <c r="G30" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="J30" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
@@ -2460,13 +2633,17 @@
         <v>2.0</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+        <v>143</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -2486,34 +2663,34 @@
     </row>
     <row r="32" ht="64.5" customHeight="1">
       <c r="A32" s="4">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F32" s="4">
         <v>1.0</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -2537,16 +2714,16 @@
         <v>2.0</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -2570,16 +2747,16 @@
         <v>3.0</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -2603,16 +2780,16 @@
         <v>4.0</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -2636,16 +2813,16 @@
         <v>5.0</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -2669,16 +2846,16 @@
         <v>6.0</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -2699,34 +2876,34 @@
     </row>
     <row r="38" ht="119.25" customHeight="1">
       <c r="A38" s="4">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F38" s="4">
         <v>1.0</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -2747,34 +2924,34 @@
     </row>
     <row r="39">
       <c r="A39" s="4">
-        <v>14.0</v>
+        <v>19.0</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F39" s="4">
         <v>1.0</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -2798,16 +2975,16 @@
         <v>2.0</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -2827,35 +3004,20 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="4">
-        <v>15.0</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="F41" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G41" s="4" t="s">
+      <c r="H41" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="I41" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -2876,34 +3038,34 @@
     </row>
     <row r="42">
       <c r="A42" s="4">
-        <v>16.0</v>
+        <v>20.0</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F42" s="4">
         <v>1.0</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -2923,20 +3085,35 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43">
+      <c r="A43" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>201</v>
+      </c>
       <c r="F43" s="4">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2956,23 +3133,8 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44">
-      <c r="A44" s="4">
-        <v>17.0</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>205</v>
-      </c>
       <c r="F44" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>206</v>
@@ -3004,20 +3166,35 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45">
+      <c r="A45" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>212</v>
+      </c>
       <c r="F45" s="4">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -3038,19 +3215,19 @@
     </row>
     <row r="46">
       <c r="F46" s="4">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -3069,36 +3246,21 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47" ht="24.0" customHeight="1">
-      <c r="A47" s="4">
-        <v>18.0</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>219</v>
-      </c>
+    <row r="47">
       <c r="F47" s="4">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>208</v>
+        <v>223</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -3117,21 +3279,36 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48" ht="25.5" customHeight="1">
+    <row r="48" ht="24.0" customHeight="1">
+      <c r="A48" s="4">
+        <v>23.0</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="F48" s="4">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -3150,21 +3327,21 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49" ht="50.25" customHeight="1">
+    <row r="49" ht="25.5" customHeight="1">
       <c r="F49" s="4">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G49" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="J49" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>223</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -3185,19 +3362,19 @@
     </row>
     <row r="50" ht="50.25" customHeight="1">
       <c r="F50" s="4">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
@@ -3216,24 +3393,9 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51">
-      <c r="A51" s="4">
-        <v>19.0</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>229</v>
-      </c>
+    <row r="51" ht="50.25" customHeight="1">
       <c r="F51" s="4">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>230</v>
@@ -3241,7 +3403,7 @@
       <c r="H51" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="I51" s="12" t="s">
         <v>232</v>
       </c>
       <c r="J51" s="4" t="s">
@@ -3266,34 +3428,34 @@
     </row>
     <row r="52">
       <c r="A52" s="4">
-        <v>20.0</v>
+        <v>24.0</v>
       </c>
       <c r="B52" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>237</v>
       </c>
       <c r="F52" s="4">
         <v>1.0</v>
       </c>
       <c r="G52" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I52" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="H52" s="12" t="s">
+      <c r="J52" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="J52" s="4" t="s">
-        <v>241</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -3313,35 +3475,20 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53">
-      <c r="A53" s="4">
-        <v>21.0</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D53" s="4" t="s">
+      <c r="F53" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="J53" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="F53" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -3361,35 +3508,20 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54">
-      <c r="A54" s="4">
-        <v>22.0</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>249</v>
-      </c>
       <c r="F54" s="4">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -3410,34 +3542,34 @@
     </row>
     <row r="55">
       <c r="A55" s="4">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>39</v>
+        <v>248</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>186</v>
+        <v>249</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F55" s="4">
         <v>1.0</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>190</v>
+        <v>252</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>253</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>191</v>
+        <v>254</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>192</v>
+        <v>255</v>
       </c>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
@@ -3457,14 +3589,14 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56">
-      <c r="A56" s="14">
-        <v>23.0</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>186</v>
+      <c r="A56" s="4">
+        <v>26.0</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>256</v>
@@ -3506,34 +3638,34 @@
     </row>
     <row r="57">
       <c r="A57" s="4">
-        <v>24.0</v>
+        <v>27.0</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C57" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="F57" s="4">
         <v>1.0</v>
       </c>
       <c r="G57" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="H57" s="4" t="s">
+      <c r="I57" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="I57" s="4" t="s">
+      <c r="J57" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>268</v>
       </c>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
@@ -3553,20 +3685,35 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58">
+      <c r="A58" s="4">
+        <v>28.0</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>269</v>
+      </c>
       <c r="F58" s="4">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>269</v>
+        <v>196</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>270</v>
+        <v>197</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>271</v>
+        <v>198</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>272</v>
+        <v>199</v>
       </c>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
@@ -3586,35 +3733,35 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59">
-      <c r="A59" s="4">
-        <v>25.0</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>262</v>
+      <c r="A59" s="14">
+        <v>29.0</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F59" s="4">
         <v>1.0</v>
       </c>
       <c r="G59" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="J59" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>278</v>
       </c>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
@@ -3633,9 +3780,24 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" ht="129.75" customHeight="1">
+    <row r="60">
+      <c r="A60" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>278</v>
+      </c>
       <c r="F60" s="4">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>279</v>
@@ -3666,36 +3828,21 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61" ht="84.75" customHeight="1">
-      <c r="A61" s="4">
-        <v>26.0</v>
-      </c>
-      <c r="B61" s="4" t="s">
+    <row r="61">
+      <c r="F61" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G61" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="I61" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="F61" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="H61" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>290</v>
       </c>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
@@ -3714,21 +3861,36 @@
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62" ht="105.75" customHeight="1">
+    <row r="62">
+      <c r="A62" s="4">
+        <v>31.0</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>288</v>
+      </c>
       <c r="F62" s="4">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G62" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="I62" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="J62" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>294</v>
       </c>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
@@ -3748,16 +3910,21 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" ht="129.75" customHeight="1">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
+      <c r="F63" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>296</v>
+      </c>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -3775,17 +3942,37 @@
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
     </row>
-    <row r="64">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
+    <row r="64" ht="84.75" customHeight="1">
+      <c r="A64" s="4">
+        <v>32.0</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F64" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>304</v>
+      </c>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
       <c r="M64" s="2"/>
@@ -3803,17 +3990,22 @@
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
     </row>
-    <row r="65">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
+    <row r="65" ht="105.75" customHeight="1">
+      <c r="F65" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>308</v>
+      </c>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
@@ -3831,17 +4023,37 @@
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
     </row>
-    <row r="66">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
+    <row r="66" ht="129.75" customHeight="1">
+      <c r="A66" s="4">
+        <v>33.0</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F66" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
@@ -3859,17 +4071,22 @@
       <c r="Y66" s="2"/>
       <c r="Z66" s="2"/>
     </row>
-    <row r="67">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
+    <row r="67" ht="129.75" customHeight="1">
+      <c r="F67" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>319</v>
+      </c>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
@@ -3887,17 +4104,22 @@
       <c r="Y67" s="2"/>
       <c r="Z67" s="2"/>
     </row>
-    <row r="68">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
+    <row r="68" ht="129.75" customHeight="1">
+      <c r="F68" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>323</v>
+      </c>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
@@ -3915,17 +4137,37 @@
       <c r="Y68" s="2"/>
       <c r="Z68" s="2"/>
     </row>
-    <row r="69">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
+    <row r="69" ht="129.75" customHeight="1">
+      <c r="A69" s="4">
+        <v>34.0</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>330</v>
+      </c>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
@@ -3943,17 +4185,22 @@
       <c r="Y69" s="2"/>
       <c r="Z69" s="2"/>
     </row>
-    <row r="70">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
+    <row r="70" ht="129.75" customHeight="1">
+      <c r="F70" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>334</v>
+      </c>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -3971,17 +4218,22 @@
       <c r="Y70" s="2"/>
       <c r="Z70" s="2"/>
     </row>
-    <row r="71">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
+    <row r="71" ht="129.75" customHeight="1">
+      <c r="F71" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>338</v>
+      </c>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -3999,17 +4251,22 @@
       <c r="Y71" s="2"/>
       <c r="Z71" s="2"/>
     </row>
-    <row r="72">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
-      <c r="J72" s="2"/>
+    <row r="72" ht="129.75" customHeight="1">
+      <c r="F72" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>342</v>
+      </c>
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
       <c r="M72" s="2"/>
@@ -4027,17 +4284,22 @@
       <c r="Y72" s="2"/>
       <c r="Z72" s="2"/>
     </row>
-    <row r="73">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
+    <row r="73" ht="129.75" customHeight="1">
+      <c r="F73" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>346</v>
+      </c>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
@@ -4055,17 +4317,22 @@
       <c r="Y73" s="2"/>
       <c r="Z73" s="2"/>
     </row>
-    <row r="74">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
+    <row r="74" ht="129.75" customHeight="1">
+      <c r="F74" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
@@ -4083,17 +4350,17 @@
       <c r="Y74" s="2"/>
       <c r="Z74" s="2"/>
     </row>
-    <row r="75">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
-      <c r="J75" s="2"/>
+    <row r="75" ht="129.75" customHeight="1">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
@@ -4111,17 +4378,17 @@
       <c r="Y75" s="2"/>
       <c r="Z75" s="2"/>
     </row>
-    <row r="76">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
+    <row r="76" ht="129.75" customHeight="1">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
       <c r="M76" s="2"/>
@@ -4139,17 +4406,17 @@
       <c r="Y76" s="2"/>
       <c r="Z76" s="2"/>
     </row>
-    <row r="77">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
+    <row r="77" ht="129.75" customHeight="1">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
@@ -30067,9 +30334,401 @@
       <c r="Y1002" s="2"/>
       <c r="Z1002" s="2"/>
     </row>
+    <row r="1003">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="2"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="2"/>
+      <c r="M1003" s="2"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="P1003" s="2"/>
+      <c r="Q1003" s="2"/>
+      <c r="R1003" s="2"/>
+      <c r="S1003" s="2"/>
+      <c r="T1003" s="2"/>
+      <c r="U1003" s="2"/>
+      <c r="V1003" s="2"/>
+      <c r="W1003" s="2"/>
+      <c r="X1003" s="2"/>
+      <c r="Y1003" s="2"/>
+      <c r="Z1003" s="2"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+      <c r="C1004" s="2"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="2"/>
+      <c r="F1004" s="2"/>
+      <c r="G1004" s="2"/>
+      <c r="H1004" s="2"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="2"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="2"/>
+      <c r="M1004" s="2"/>
+      <c r="N1004" s="2"/>
+      <c r="O1004" s="2"/>
+      <c r="P1004" s="2"/>
+      <c r="Q1004" s="2"/>
+      <c r="R1004" s="2"/>
+      <c r="S1004" s="2"/>
+      <c r="T1004" s="2"/>
+      <c r="U1004" s="2"/>
+      <c r="V1004" s="2"/>
+      <c r="W1004" s="2"/>
+      <c r="X1004" s="2"/>
+      <c r="Y1004" s="2"/>
+      <c r="Z1004" s="2"/>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="2"/>
+      <c r="B1005" s="2"/>
+      <c r="C1005" s="2"/>
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="2"/>
+      <c r="F1005" s="2"/>
+      <c r="G1005" s="2"/>
+      <c r="H1005" s="2"/>
+      <c r="I1005" s="2"/>
+      <c r="J1005" s="2"/>
+      <c r="K1005" s="2"/>
+      <c r="L1005" s="2"/>
+      <c r="M1005" s="2"/>
+      <c r="N1005" s="2"/>
+      <c r="O1005" s="2"/>
+      <c r="P1005" s="2"/>
+      <c r="Q1005" s="2"/>
+      <c r="R1005" s="2"/>
+      <c r="S1005" s="2"/>
+      <c r="T1005" s="2"/>
+      <c r="U1005" s="2"/>
+      <c r="V1005" s="2"/>
+      <c r="W1005" s="2"/>
+      <c r="X1005" s="2"/>
+      <c r="Y1005" s="2"/>
+      <c r="Z1005" s="2"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="2"/>
+      <c r="B1006" s="2"/>
+      <c r="C1006" s="2"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="2"/>
+      <c r="F1006" s="2"/>
+      <c r="G1006" s="2"/>
+      <c r="H1006" s="2"/>
+      <c r="I1006" s="2"/>
+      <c r="J1006" s="2"/>
+      <c r="K1006" s="2"/>
+      <c r="L1006" s="2"/>
+      <c r="M1006" s="2"/>
+      <c r="N1006" s="2"/>
+      <c r="O1006" s="2"/>
+      <c r="P1006" s="2"/>
+      <c r="Q1006" s="2"/>
+      <c r="R1006" s="2"/>
+      <c r="S1006" s="2"/>
+      <c r="T1006" s="2"/>
+      <c r="U1006" s="2"/>
+      <c r="V1006" s="2"/>
+      <c r="W1006" s="2"/>
+      <c r="X1006" s="2"/>
+      <c r="Y1006" s="2"/>
+      <c r="Z1006" s="2"/>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="2"/>
+      <c r="B1007" s="2"/>
+      <c r="C1007" s="2"/>
+      <c r="D1007" s="2"/>
+      <c r="E1007" s="2"/>
+      <c r="F1007" s="2"/>
+      <c r="G1007" s="2"/>
+      <c r="H1007" s="2"/>
+      <c r="I1007" s="2"/>
+      <c r="J1007" s="2"/>
+      <c r="K1007" s="2"/>
+      <c r="L1007" s="2"/>
+      <c r="M1007" s="2"/>
+      <c r="N1007" s="2"/>
+      <c r="O1007" s="2"/>
+      <c r="P1007" s="2"/>
+      <c r="Q1007" s="2"/>
+      <c r="R1007" s="2"/>
+      <c r="S1007" s="2"/>
+      <c r="T1007" s="2"/>
+      <c r="U1007" s="2"/>
+      <c r="V1007" s="2"/>
+      <c r="W1007" s="2"/>
+      <c r="X1007" s="2"/>
+      <c r="Y1007" s="2"/>
+      <c r="Z1007" s="2"/>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="2"/>
+      <c r="B1008" s="2"/>
+      <c r="C1008" s="2"/>
+      <c r="D1008" s="2"/>
+      <c r="E1008" s="2"/>
+      <c r="F1008" s="2"/>
+      <c r="G1008" s="2"/>
+      <c r="H1008" s="2"/>
+      <c r="I1008" s="2"/>
+      <c r="J1008" s="2"/>
+      <c r="K1008" s="2"/>
+      <c r="L1008" s="2"/>
+      <c r="M1008" s="2"/>
+      <c r="N1008" s="2"/>
+      <c r="O1008" s="2"/>
+      <c r="P1008" s="2"/>
+      <c r="Q1008" s="2"/>
+      <c r="R1008" s="2"/>
+      <c r="S1008" s="2"/>
+      <c r="T1008" s="2"/>
+      <c r="U1008" s="2"/>
+      <c r="V1008" s="2"/>
+      <c r="W1008" s="2"/>
+      <c r="X1008" s="2"/>
+      <c r="Y1008" s="2"/>
+      <c r="Z1008" s="2"/>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="2"/>
+      <c r="B1009" s="2"/>
+      <c r="C1009" s="2"/>
+      <c r="D1009" s="2"/>
+      <c r="E1009" s="2"/>
+      <c r="F1009" s="2"/>
+      <c r="G1009" s="2"/>
+      <c r="H1009" s="2"/>
+      <c r="I1009" s="2"/>
+      <c r="J1009" s="2"/>
+      <c r="K1009" s="2"/>
+      <c r="L1009" s="2"/>
+      <c r="M1009" s="2"/>
+      <c r="N1009" s="2"/>
+      <c r="O1009" s="2"/>
+      <c r="P1009" s="2"/>
+      <c r="Q1009" s="2"/>
+      <c r="R1009" s="2"/>
+      <c r="S1009" s="2"/>
+      <c r="T1009" s="2"/>
+      <c r="U1009" s="2"/>
+      <c r="V1009" s="2"/>
+      <c r="W1009" s="2"/>
+      <c r="X1009" s="2"/>
+      <c r="Y1009" s="2"/>
+      <c r="Z1009" s="2"/>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="2"/>
+      <c r="B1010" s="2"/>
+      <c r="C1010" s="2"/>
+      <c r="D1010" s="2"/>
+      <c r="E1010" s="2"/>
+      <c r="F1010" s="2"/>
+      <c r="G1010" s="2"/>
+      <c r="H1010" s="2"/>
+      <c r="I1010" s="2"/>
+      <c r="J1010" s="2"/>
+      <c r="K1010" s="2"/>
+      <c r="L1010" s="2"/>
+      <c r="M1010" s="2"/>
+      <c r="N1010" s="2"/>
+      <c r="O1010" s="2"/>
+      <c r="P1010" s="2"/>
+      <c r="Q1010" s="2"/>
+      <c r="R1010" s="2"/>
+      <c r="S1010" s="2"/>
+      <c r="T1010" s="2"/>
+      <c r="U1010" s="2"/>
+      <c r="V1010" s="2"/>
+      <c r="W1010" s="2"/>
+      <c r="X1010" s="2"/>
+      <c r="Y1010" s="2"/>
+      <c r="Z1010" s="2"/>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="2"/>
+      <c r="B1011" s="2"/>
+      <c r="C1011" s="2"/>
+      <c r="D1011" s="2"/>
+      <c r="E1011" s="2"/>
+      <c r="F1011" s="2"/>
+      <c r="G1011" s="2"/>
+      <c r="H1011" s="2"/>
+      <c r="I1011" s="2"/>
+      <c r="J1011" s="2"/>
+      <c r="K1011" s="2"/>
+      <c r="L1011" s="2"/>
+      <c r="M1011" s="2"/>
+      <c r="N1011" s="2"/>
+      <c r="O1011" s="2"/>
+      <c r="P1011" s="2"/>
+      <c r="Q1011" s="2"/>
+      <c r="R1011" s="2"/>
+      <c r="S1011" s="2"/>
+      <c r="T1011" s="2"/>
+      <c r="U1011" s="2"/>
+      <c r="V1011" s="2"/>
+      <c r="W1011" s="2"/>
+      <c r="X1011" s="2"/>
+      <c r="Y1011" s="2"/>
+      <c r="Z1011" s="2"/>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="2"/>
+      <c r="B1012" s="2"/>
+      <c r="C1012" s="2"/>
+      <c r="D1012" s="2"/>
+      <c r="E1012" s="2"/>
+      <c r="F1012" s="2"/>
+      <c r="G1012" s="2"/>
+      <c r="H1012" s="2"/>
+      <c r="I1012" s="2"/>
+      <c r="J1012" s="2"/>
+      <c r="K1012" s="2"/>
+      <c r="L1012" s="2"/>
+      <c r="M1012" s="2"/>
+      <c r="N1012" s="2"/>
+      <c r="O1012" s="2"/>
+      <c r="P1012" s="2"/>
+      <c r="Q1012" s="2"/>
+      <c r="R1012" s="2"/>
+      <c r="S1012" s="2"/>
+      <c r="T1012" s="2"/>
+      <c r="U1012" s="2"/>
+      <c r="V1012" s="2"/>
+      <c r="W1012" s="2"/>
+      <c r="X1012" s="2"/>
+      <c r="Y1012" s="2"/>
+      <c r="Z1012" s="2"/>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="2"/>
+      <c r="B1013" s="2"/>
+      <c r="C1013" s="2"/>
+      <c r="D1013" s="2"/>
+      <c r="E1013" s="2"/>
+      <c r="F1013" s="2"/>
+      <c r="G1013" s="2"/>
+      <c r="H1013" s="2"/>
+      <c r="I1013" s="2"/>
+      <c r="J1013" s="2"/>
+      <c r="K1013" s="2"/>
+      <c r="L1013" s="2"/>
+      <c r="M1013" s="2"/>
+      <c r="N1013" s="2"/>
+      <c r="O1013" s="2"/>
+      <c r="P1013" s="2"/>
+      <c r="Q1013" s="2"/>
+      <c r="R1013" s="2"/>
+      <c r="S1013" s="2"/>
+      <c r="T1013" s="2"/>
+      <c r="U1013" s="2"/>
+      <c r="V1013" s="2"/>
+      <c r="W1013" s="2"/>
+      <c r="X1013" s="2"/>
+      <c r="Y1013" s="2"/>
+      <c r="Z1013" s="2"/>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="2"/>
+      <c r="B1014" s="2"/>
+      <c r="C1014" s="2"/>
+      <c r="D1014" s="2"/>
+      <c r="E1014" s="2"/>
+      <c r="F1014" s="2"/>
+      <c r="G1014" s="2"/>
+      <c r="H1014" s="2"/>
+      <c r="I1014" s="2"/>
+      <c r="J1014" s="2"/>
+      <c r="K1014" s="2"/>
+      <c r="L1014" s="2"/>
+      <c r="M1014" s="2"/>
+      <c r="N1014" s="2"/>
+      <c r="O1014" s="2"/>
+      <c r="P1014" s="2"/>
+      <c r="Q1014" s="2"/>
+      <c r="R1014" s="2"/>
+      <c r="S1014" s="2"/>
+      <c r="T1014" s="2"/>
+      <c r="U1014" s="2"/>
+      <c r="V1014" s="2"/>
+      <c r="W1014" s="2"/>
+      <c r="X1014" s="2"/>
+      <c r="Y1014" s="2"/>
+      <c r="Z1014" s="2"/>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="2"/>
+      <c r="B1015" s="2"/>
+      <c r="C1015" s="2"/>
+      <c r="D1015" s="2"/>
+      <c r="E1015" s="2"/>
+      <c r="F1015" s="2"/>
+      <c r="G1015" s="2"/>
+      <c r="H1015" s="2"/>
+      <c r="I1015" s="2"/>
+      <c r="J1015" s="2"/>
+      <c r="K1015" s="2"/>
+      <c r="L1015" s="2"/>
+      <c r="M1015" s="2"/>
+      <c r="N1015" s="2"/>
+      <c r="O1015" s="2"/>
+      <c r="P1015" s="2"/>
+      <c r="Q1015" s="2"/>
+      <c r="R1015" s="2"/>
+      <c r="S1015" s="2"/>
+      <c r="T1015" s="2"/>
+      <c r="U1015" s="2"/>
+      <c r="V1015" s="2"/>
+      <c r="W1015" s="2"/>
+      <c r="X1015" s="2"/>
+      <c r="Y1015" s="2"/>
+      <c r="Z1015" s="2"/>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="2"/>
+      <c r="B1016" s="2"/>
+      <c r="C1016" s="2"/>
+      <c r="D1016" s="2"/>
+      <c r="E1016" s="2"/>
+      <c r="F1016" s="2"/>
+      <c r="G1016" s="2"/>
+      <c r="H1016" s="2"/>
+      <c r="I1016" s="2"/>
+      <c r="J1016" s="2"/>
+      <c r="K1016" s="2"/>
+      <c r="L1016" s="2"/>
+      <c r="M1016" s="2"/>
+      <c r="N1016" s="2"/>
+      <c r="O1016" s="2"/>
+      <c r="P1016" s="2"/>
+      <c r="Q1016" s="2"/>
+      <c r="R1016" s="2"/>
+      <c r="S1016" s="2"/>
+      <c r="T1016" s="2"/>
+      <c r="U1016" s="2"/>
+      <c r="V1016" s="2"/>
+      <c r="W1016" s="2"/>
+      <c r="X1016" s="2"/>
+      <c r="Y1016" s="2"/>
+      <c r="Z1016" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$B$2:$J$62"/>
-  <mergeCells count="88">
+  <autoFilter ref="$A$2:$J$74"/>
+  <mergeCells count="104">
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
@@ -30085,35 +30744,54 @@
     <mergeCell ref="C32:C37"/>
     <mergeCell ref="D32:D37"/>
     <mergeCell ref="E32:E37"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="B69:B74"/>
+    <mergeCell ref="C69:C74"/>
+    <mergeCell ref="D69:D74"/>
+    <mergeCell ref="E69:E74"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A74"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="A3:A4"/>
@@ -30139,12 +30817,12 @@
     <mergeCell ref="I20:I21"/>
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="D14:D18"/>
     <mergeCell ref="E14:E18"/>
-    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A18"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A22:A23"/>
@@ -30152,12 +30830,9 @@
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>